<commit_message>
add: add cls result
</commit_message>
<xml_diff>
--- a/results/ML_All/Tx(K)_ml.xlsx
+++ b/results/ML_All/Tx(K)_ml.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -493,22 +493,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'alpha': 100, 'max_iter': 1000}</t>
+          <t>{'alpha': 0.1, 'max_iter': 1000}</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'alpha': 1, 'max_iter': 1000}</t>
+          <t>{'alpha': 0.001, 'max_iter': 1000}</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{'alpha': 1, 'l1_ratio': 0.75, 'max_iter': 1000}</t>
+          <t>{'alpha': 0.001, 'l1_ratio': 0.25, 'max_iter': 1000}</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>{'C': 100, 'gamma': 0.01}</t>
+          <t>{'C': 1, 'gamma': 1}</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{'activation': 'leaky_relu', 'b_random_vec_range': [0, 10], 'lam': 1, 'n_layer': 32, 'n_nodes': 256, 'random_seed': 9, 'same_feature': True, 'w_random_vec_range': [-10, 10]}</t>
+          <t>{'activation': 'relu', 'b_random_vec_range': [0, 10], 'lam': 1, 'n_layer': 16, 'n_nodes': 256, 'random_seed': 358, 'same_feature': True, 'w_random_vec_range': [-10, 10]}</t>
         </is>
       </c>
     </row>
@@ -549,34 +549,34 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>53.892239594594</v>
+        <v>0.07365191382727573</v>
       </c>
       <c r="C3" t="n">
-        <v>53.55560148360023</v>
+        <v>0.09482543562865793</v>
       </c>
       <c r="D3" t="n">
-        <v>53.67263855697056</v>
+        <v>0.0822952872556722</v>
       </c>
       <c r="E3" t="n">
-        <v>61.64460398426233</v>
+        <v>0.07614074535858557</v>
       </c>
       <c r="F3" t="n">
-        <v>43.03092789854885</v>
+        <v>0.05290137422467665</v>
       </c>
       <c r="G3" t="n">
-        <v>40.2901760330902</v>
+        <v>0.05019867482937072</v>
       </c>
       <c r="H3" t="n">
-        <v>73.91912408451074</v>
+        <v>0.1015212474423683</v>
       </c>
       <c r="I3" t="n">
-        <v>34.38477389373483</v>
+        <v>0.04719998031908251</v>
       </c>
       <c r="J3" t="n">
-        <v>39.1976720037386</v>
+        <v>0.05070881903069058</v>
       </c>
       <c r="K3" t="n">
-        <v>18.48122147525931</v>
+        <v>0.02673389891972606</v>
       </c>
     </row>
     <row r="4">
@@ -586,34 +586,34 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.904531526996999</v>
+        <v>0.9049519609820754</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9061839710161153</v>
+        <v>0.8423433234817181</v>
       </c>
       <c r="D4" t="n">
-        <v>0.905502956981629</v>
+        <v>0.881720028899452</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8785494484251106</v>
+        <v>0.8988318188252457</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9398250257175669</v>
+        <v>0.9483827196779414</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9480633980963649</v>
+        <v>0.953396796924791</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8273754374495874</v>
+        <v>0.8230625889627975</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9613453951195897</v>
+        <v>0.9595943643042307</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9495120638859105</v>
+        <v>0.9542264983691717</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9880475188966968</v>
+        <v>0.986653353629201</v>
       </c>
     </row>
     <row r="5">
@@ -623,34 +623,34 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.606968154995181</v>
+        <v>13.20094430097138</v>
       </c>
       <c r="C5" t="n">
-        <v>5.580773771212359</v>
+        <v>17.97304476803705</v>
       </c>
       <c r="D5" t="n">
-        <v>5.615673863905679</v>
+        <v>15.27312564475146</v>
       </c>
       <c r="E5" t="n">
-        <v>6.292557819303328</v>
+        <v>16.13094892244744</v>
       </c>
       <c r="F5" t="n">
-        <v>3.286793018479254</v>
+        <v>6.427331223082751</v>
       </c>
       <c r="G5" t="n">
-        <v>3.13722971993793</v>
+        <v>6.371517571339483</v>
       </c>
       <c r="H5" t="n">
-        <v>8.717951697365933</v>
+        <v>19.40265142933292</v>
       </c>
       <c r="I5" t="n">
-        <v>2.76945167497709</v>
+        <v>6.296702272859105</v>
       </c>
       <c r="J5" t="n">
-        <v>3.332027740681056</v>
+        <v>7.175632936858507</v>
       </c>
       <c r="K5" t="n">
-        <v>1.81820516356686</v>
+        <v>3.774573562720013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>